<commit_message>
finish repairing d18O issue by reverting to previous commit
</commit_message>
<xml_diff>
--- a/src/example_scrambling_output.xlsx
+++ b/src/example_scrambling_output.xlsx
@@ -519,16 +519,16 @@
         <v>0.003768911734945011</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007790613819287051</v>
+        <v>0.007793499819165031</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002117490233832286</v>
+        <v>0.002116479886116219</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003703019004167107</v>
+        <v>0.003702170629356947</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0003845742699228161</v>
+        <v>0.0003891569923179599</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -539,22 +539,22 @@
         <v>0.003722801775248976</v>
       </c>
       <c r="J2" t="n">
-        <v>0.007743991908667606</v>
+        <v>0.007744164034237219</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002110353165636288</v>
+        <v>0.002109788966545483</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003680040562593211</v>
+        <v>0.003677820676590643</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0003839107441448915</v>
+        <v>0.0003885226687727657</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2091288397435046</v>
+        <v>0.2089187583979959</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1176061290839624</v>
+        <v>0.1161406344584892</v>
       </c>
     </row>
     <row r="3">
@@ -570,16 +570,16 @@
         <v>0.003768911734945011</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007790613819287051</v>
+        <v>0.007793499819165031</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002117490233832286</v>
+        <v>0.002116479886116219</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003703019004167107</v>
+        <v>0.003702170629356947</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003845742699228161</v>
+        <v>0.0003891569923179599</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -590,22 +590,22 @@
         <v>0.003719928535364826</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00773460518481109</v>
+        <v>0.007734232986583432</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002106309102767537</v>
+        <v>0.002105997079923158</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003675538503072143</v>
+        <v>0.003673038475728314</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0003835281810239039</v>
+        <v>0.0003881560437870166</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1740326254061542</v>
+        <v>0.1735976339601624</v>
       </c>
       <c r="O3" t="n">
-        <v>0.08184087885576256</v>
+        <v>0.08014618668934347</v>
       </c>
     </row>
     <row r="4">
@@ -621,16 +621,16 @@
         <v>0.003770760540076305</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007780458901723035</v>
+        <v>0.007782752318650127</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002113297007446234</v>
+        <v>0.002112548954645945</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003698140054633031</v>
+        <v>0.003696987095268748</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0003841777559768219</v>
+        <v>0.000388777098467939</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -641,22 +641,22 @@
         <v>0.003722801775248976</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007743991908667606</v>
+        <v>0.007744164034237219</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002110353165636288</v>
+        <v>0.002109788966545483</v>
       </c>
       <c r="L4" t="n">
-        <v>0.003680040562593211</v>
+        <v>0.003677820676590643</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0003839107441448915</v>
+        <v>0.0003885226687727657</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1773914372444855</v>
+        <v>0.1774159913196851</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08587684673364403</v>
+        <v>0.08464592749641378</v>
       </c>
     </row>
     <row r="5">
@@ -672,16 +672,16 @@
         <v>0.003770760540076305</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007780458901723035</v>
+        <v>0.007782752318650127</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002113297007446234</v>
+        <v>0.002112548954645945</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003698140054633031</v>
+        <v>0.003696987095268748</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003841777559768219</v>
+        <v>0.000388777098467939</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -692,22 +692,22 @@
         <v>0.003719928535364826</v>
       </c>
       <c r="J5" t="n">
-        <v>0.00773460518481109</v>
+        <v>0.007734232986583432</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002106309102767537</v>
+        <v>0.002105997079923158</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003675538503072143</v>
+        <v>0.003673038475728314</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0003835281810239039</v>
+        <v>0.0003881560437870166</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1422952229071351</v>
+        <v>0.1420948668818515</v>
       </c>
       <c r="O5" t="n">
-        <v>0.05011159650544415</v>
+        <v>0.04865147972726809</v>
       </c>
     </row>
     <row r="6">
@@ -723,16 +723,16 @@
         <v>0.003774157409185728</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007785298049737537</v>
+        <v>0.007787873750271767</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002112773739538533</v>
+        <v>0.00211205838421125</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003700585433254881</v>
+        <v>0.003699572671149732</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000384125912537138</v>
+        <v>0.0003887271293238374</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -743,22 +743,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N6" t="n">
-        <v>0.150009511853521</v>
+        <v>0.1500279247660436</v>
       </c>
       <c r="O6" t="n">
-        <v>0.05891467380941966</v>
+        <v>0.05767699316230707</v>
       </c>
     </row>
     <row r="7">
@@ -774,16 +774,16 @@
         <v>0.003766158719891302</v>
       </c>
       <c r="D7" t="n">
-        <v>0.007778805439255057</v>
+        <v>0.007781002446557233</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002112558106649536</v>
+        <v>0.002111856223390097</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003697348321425102</v>
+        <v>0.003696145699730478</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0003841078325232079</v>
+        <v>0.0003887100943970135</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -794,22 +794,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2628146441537145</v>
+        <v>0.2628488641090769</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1716909444392702</v>
+        <v>0.1704690667906986</v>
       </c>
     </row>
     <row r="8">
@@ -825,16 +825,16 @@
         <v>0.003773012631577434</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007784674507108374</v>
+        <v>0.007787213823960496</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002114885674162161</v>
+        <v>0.002114038303996214</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00370017271711588</v>
+        <v>0.00369914585293415</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0003843278386694184</v>
+        <v>0.0003889208781295111</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -845,22 +845,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J8" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1690449117708085</v>
+        <v>0.1689479131022625</v>
       </c>
       <c r="O8" t="n">
-        <v>0.07794520343910534</v>
+        <v>0.07659214073946548</v>
       </c>
     </row>
   </sheetData>
@@ -972,16 +972,16 @@
         <v>0.003768911734945011</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007790613819287051</v>
+        <v>0.007793499819165031</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002117490233832286</v>
+        <v>0.002116479886116219</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003703019004167107</v>
+        <v>0.003702170629356947</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0003845742699228161</v>
+        <v>0.0003891569923179599</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -992,22 +992,22 @@
         <v>0.003722801775248976</v>
       </c>
       <c r="J2" t="n">
-        <v>0.007743991908667606</v>
+        <v>0.007744164034237219</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002110353165636288</v>
+        <v>0.002109788966545483</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003680040562593211</v>
+        <v>0.003677820676590643</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0003839107441448915</v>
+        <v>0.0003885226687727657</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2091288397435046</v>
+        <v>0.2089187583979959</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1176061290839624</v>
+        <v>0.1161406344584892</v>
       </c>
     </row>
     <row r="3">
@@ -1023,16 +1023,16 @@
         <v>0.003768911734945011</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007790613819287051</v>
+        <v>0.007793499819165031</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002117490233832286</v>
+        <v>0.002116479886116219</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003703019004167107</v>
+        <v>0.003702170629356947</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003845742699228161</v>
+        <v>0.0003891569923179599</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1043,22 +1043,22 @@
         <v>0.003719928535364826</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00773460518481109</v>
+        <v>0.007734232986583432</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002106309102767537</v>
+        <v>0.002105997079923158</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003675538503072143</v>
+        <v>0.003673038475728314</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0003835281810239039</v>
+        <v>0.0003881560437870166</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1740326254061542</v>
+        <v>0.1735976339601624</v>
       </c>
       <c r="O3" t="n">
-        <v>0.08184087885576256</v>
+        <v>0.08014618668934347</v>
       </c>
     </row>
     <row r="4">
@@ -1074,16 +1074,16 @@
         <v>0.003770760540076305</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007780458901723035</v>
+        <v>0.007782752318650127</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002113297007446234</v>
+        <v>0.002112548954645945</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003698140054633031</v>
+        <v>0.003696987095268748</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0003841777559768219</v>
+        <v>0.000388777098467939</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1094,22 +1094,22 @@
         <v>0.003722801775248976</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007743991908667606</v>
+        <v>0.007744164034237219</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002110353165636288</v>
+        <v>0.002109788966545483</v>
       </c>
       <c r="L4" t="n">
-        <v>0.003680040562593211</v>
+        <v>0.003677820676590643</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0003839107441448915</v>
+        <v>0.0003885226687727657</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1773914372444855</v>
+        <v>0.1774159913196851</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08587684673364403</v>
+        <v>0.08464592749641378</v>
       </c>
     </row>
     <row r="5">
@@ -1125,16 +1125,16 @@
         <v>0.003770760540076305</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007780458901723035</v>
+        <v>0.007782752318650127</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002113297007446234</v>
+        <v>0.002112548954645945</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003698140054633031</v>
+        <v>0.003696987095268748</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003841777559768219</v>
+        <v>0.000388777098467939</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1145,22 +1145,22 @@
         <v>0.003719928535364826</v>
       </c>
       <c r="J5" t="n">
-        <v>0.00773460518481109</v>
+        <v>0.007734232986583432</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002106309102767537</v>
+        <v>0.002105997079923158</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003675538503072143</v>
+        <v>0.003673038475728314</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0003835281810239039</v>
+        <v>0.0003881560437870166</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1422952229071351</v>
+        <v>0.1420948668818515</v>
       </c>
       <c r="O5" t="n">
-        <v>0.05011159650544415</v>
+        <v>0.04865147972726809</v>
       </c>
     </row>
     <row r="6">
@@ -1176,16 +1176,16 @@
         <v>0.003774157409185728</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007785298049737537</v>
+        <v>0.007787873750271767</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002112773739538533</v>
+        <v>0.00211205838421125</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003700585433254881</v>
+        <v>0.003699572671149732</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000384125912537138</v>
+        <v>0.0003887271293238374</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1196,22 +1196,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N6" t="n">
-        <v>0.150009511853521</v>
+        <v>0.1500279247660436</v>
       </c>
       <c r="O6" t="n">
-        <v>0.05891467380941966</v>
+        <v>0.05767699316230707</v>
       </c>
     </row>
     <row r="7">
@@ -1227,16 +1227,16 @@
         <v>0.003766158719891302</v>
       </c>
       <c r="D7" t="n">
-        <v>0.007778805439255057</v>
+        <v>0.007781002446557233</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002112558106649536</v>
+        <v>0.002111856223390097</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003697348321425102</v>
+        <v>0.003696145699730478</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0003841078325232079</v>
+        <v>0.0003887100943970135</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1247,22 +1247,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2628146441537145</v>
+        <v>0.2628488641090769</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1716909444392702</v>
+        <v>0.1704690667906986</v>
       </c>
     </row>
     <row r="8">
@@ -1278,16 +1278,16 @@
         <v>0.003773012631577434</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007784674507108374</v>
+        <v>0.007787213823960496</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002114885674162161</v>
+        <v>0.002114038303996214</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00370017271711588</v>
+        <v>0.00369914585293415</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0003843278386694184</v>
+        <v>0.0003889208781295111</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1298,22 +1298,22 @@
         <v>0.003724263165303106</v>
       </c>
       <c r="J8" t="n">
-        <v>0.007742415894486522</v>
+        <v>0.007742496580265385</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002109772591168823</v>
+        <v>0.002109244622837149</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003679279978564898</v>
+        <v>0.003677013222209626</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0003838559110058119</v>
+        <v>0.0003884701338024097</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1690449117708085</v>
+        <v>0.1689479131022625</v>
       </c>
       <c r="O8" t="n">
-        <v>0.07794520343910534</v>
+        <v>0.07659214073946548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
needed to change scramblinginput.py so that it was referencing the right column as 17R
</commit_message>
<xml_diff>
--- a/src/example_scrambling_output.xlsx
+++ b/src/example_scrambling_output.xlsx
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003768911734945011</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007793499819165031</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002116479886116219</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003702222127051057</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G2" t="n">
-        <v>0.002099893460859661</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -536,25 +536,25 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.003722801775248976</v>
+        <v>0.003723787788712729</v>
       </c>
       <c r="J2" t="n">
-        <v>0.007744164034237219</v>
+        <v>0.007744018133863363</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002109788966545483</v>
+        <v>0.002106521197767294</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003677865467017766</v>
+        <v>0.003677948519669682</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00209340517209855</v>
+        <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3670017863326024</v>
+        <v>0.2084769676046654</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.1907152885455783</v>
+        <v>0.1160767438553549</v>
       </c>
     </row>
     <row r="3">
@@ -567,19 +567,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.003768911734945011</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007793499819165031</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002116479886116219</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003702222127051057</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002099893460859661</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -587,25 +587,25 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.003719928535364826</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J3" t="n">
-        <v>0.007734232986583432</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002105997079923158</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003673082346325243</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M3" t="n">
-        <v>0.002089664688983711</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N3" t="n">
-        <v>0.379263849191313</v>
+        <v>0.173005804283726</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.1782194751156673</v>
+        <v>0.07992939702573887</v>
       </c>
     </row>
     <row r="4">
@@ -618,19 +618,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.003770760540076305</v>
+        <v>0.003771759255797842</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007782752318650127</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002112548954645945</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003697034627764989</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002096007444871974</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -638,25 +638,25 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.003722801775248976</v>
+        <v>0.003723787788712729</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007744164034237219</v>
+        <v>0.007744018133863363</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002109788966545483</v>
+        <v>0.002106521197767294</v>
       </c>
       <c r="L4" t="n">
-        <v>0.003677865467017766</v>
+        <v>0.003677948519669682</v>
       </c>
       <c r="M4" t="n">
-        <v>0.00209340517209855</v>
+        <v>0.0003881208956607774</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2856629739041236</v>
+        <v>0.1770877874050666</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.2720332900947778</v>
+        <v>0.08469559471030816</v>
       </c>
     </row>
     <row r="5">
@@ -669,19 +669,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003770760540076305</v>
+        <v>0.003771759255797842</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007782752318650127</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002112548954645945</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003697034627764989</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002096007444871974</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -689,25 +689,25 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.003719928535364826</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J5" t="n">
-        <v>0.007734232986583432</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002105997079923158</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003673082346325243</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M5" t="n">
-        <v>0.002089664688983711</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2979250367628342</v>
+        <v>0.141616624084127</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.2595374766648668</v>
+        <v>0.04854824788069214</v>
       </c>
     </row>
     <row r="6">
@@ -720,19 +720,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003774157409185728</v>
+        <v>0.003775157024594888</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007787873750271767</v>
+        <v>0.007787727026405036</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00211205838421125</v>
+        <v>0.002108787100421698</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003699619699356788</v>
+        <v>0.003699702839221671</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002095496242379899</v>
+        <v>0.000388320234647194</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -740,25 +740,25 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M6" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2584883145367431</v>
+        <v>0.1496888401862124</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.2986551597096462</v>
+        <v>0.0577155186099103</v>
       </c>
     </row>
     <row r="7">
@@ -771,19 +771,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.003766158719891302</v>
+        <v>0.003767156216784404</v>
       </c>
       <c r="D7" t="n">
-        <v>0.007781002446557233</v>
+        <v>0.007780855852146149</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002111856223390097</v>
+        <v>0.002108585252719454</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003696192533421012</v>
+        <v>0.003696275723234606</v>
       </c>
       <c r="G7" t="n">
-        <v>0.002095322040949255</v>
+        <v>0.0003883035805857967</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -791,25 +791,25 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3694649080647032</v>
+        <v>0.2625447922510269</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.1877069600126482</v>
+        <v>0.1705425960019301</v>
       </c>
     </row>
     <row r="8">
@@ -822,19 +822,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.003773012631577434</v>
+        <v>0.003774011943783199</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007787213823960496</v>
+        <v>0.007787067112526803</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002114038303996214</v>
+        <v>0.002110763953587128</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003699194886987533</v>
+        <v>0.003699278179158993</v>
       </c>
       <c r="G8" t="n">
-        <v>0.002097478198739332</v>
+        <v>0.0003885097115356922</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -842,25 +842,25 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J8" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M8" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3028353265431929</v>
+        <v>0.1685526780378239</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.254319494073837</v>
+        <v>0.0765745300688003</v>
       </c>
     </row>
   </sheetData>
@@ -969,19 +969,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003768911734945011</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007793499819165031</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002116479886116219</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003702222127051057</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G2" t="n">
-        <v>0.002099893460859661</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -989,25 +989,25 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.003722801775248976</v>
+        <v>0.003723787788712729</v>
       </c>
       <c r="J2" t="n">
-        <v>0.007744164034237219</v>
+        <v>0.007744018133863363</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002109788966545483</v>
+        <v>0.002106521197767294</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003677865467017766</v>
+        <v>0.003677948519669682</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00209340517209855</v>
+        <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3670017863326024</v>
+        <v>0.2084769676046654</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.1907152885455783</v>
+        <v>0.1160767438553549</v>
       </c>
     </row>
     <row r="3">
@@ -1020,19 +1020,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.003768911734945011</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007793499819165031</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002116479886116219</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003702222127051057</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002099893460859661</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1040,25 +1040,25 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.003719928535364826</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J3" t="n">
-        <v>0.007734232986583432</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002105997079923158</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003673082346325243</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M3" t="n">
-        <v>0.002089664688983711</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N3" t="n">
-        <v>0.379263849191313</v>
+        <v>0.173005804283726</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.1782194751156673</v>
+        <v>0.07992939702573887</v>
       </c>
     </row>
     <row r="4">
@@ -1071,19 +1071,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.003770760540076305</v>
+        <v>0.003771759255797842</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007782752318650127</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002112548954645945</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003697034627764989</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002096007444871974</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1091,25 +1091,25 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.003722801775248976</v>
+        <v>0.003723787788712729</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007744164034237219</v>
+        <v>0.007744018133863363</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002109788966545483</v>
+        <v>0.002106521197767294</v>
       </c>
       <c r="L4" t="n">
-        <v>0.003677865467017766</v>
+        <v>0.003677948519669682</v>
       </c>
       <c r="M4" t="n">
-        <v>0.00209340517209855</v>
+        <v>0.0003881208956607774</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2856629739041236</v>
+        <v>0.1770877874050666</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.2720332900947778</v>
+        <v>0.08469559471030816</v>
       </c>
     </row>
     <row r="5">
@@ -1122,19 +1122,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003770760540076305</v>
+        <v>0.003771759255797842</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007782752318650127</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002112548954645945</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003697034627764989</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002096007444871974</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -1142,25 +1142,25 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.003719928535364826</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J5" t="n">
-        <v>0.007734232986583432</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002105997079923158</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003673082346325243</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M5" t="n">
-        <v>0.002089664688983711</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2979250367628342</v>
+        <v>0.141616624084127</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.2595374766648668</v>
+        <v>0.04854824788069214</v>
       </c>
     </row>
     <row r="6">
@@ -1173,19 +1173,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003774157409185728</v>
+        <v>0.003775157024594888</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007787873750271767</v>
+        <v>0.007787727026405036</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00211205838421125</v>
+        <v>0.002108787100421698</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003699619699356788</v>
+        <v>0.003699702839221671</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002095496242379899</v>
+        <v>0.000388320234647194</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -1193,25 +1193,25 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M6" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2584883145367431</v>
+        <v>0.1496888401862124</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.2986551597096462</v>
+        <v>0.0577155186099103</v>
       </c>
     </row>
     <row r="7">
@@ -1224,19 +1224,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.003766158719891302</v>
+        <v>0.003767156216784404</v>
       </c>
       <c r="D7" t="n">
-        <v>0.007781002446557233</v>
+        <v>0.007780855852146149</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002111856223390097</v>
+        <v>0.002108585252719454</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003696192533421012</v>
+        <v>0.003696275723234606</v>
       </c>
       <c r="G7" t="n">
-        <v>0.002095322040949255</v>
+        <v>0.0003883035805857967</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1244,25 +1244,25 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3694649080647032</v>
+        <v>0.2625447922510269</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.1877069600126482</v>
+        <v>0.1705425960019301</v>
       </c>
     </row>
     <row r="8">
@@ -1275,19 +1275,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.003773012631577434</v>
+        <v>0.003774011943783199</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007787213823960496</v>
+        <v>0.007787067112526803</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002114038303996214</v>
+        <v>0.002110763953587128</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003699194886987533</v>
+        <v>0.003699278179158993</v>
       </c>
       <c r="G8" t="n">
-        <v>0.002097478198739332</v>
+        <v>0.0003885097115356922</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1295,25 +1295,25 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0.003724263165303106</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J8" t="n">
-        <v>0.007742496580265385</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K8" t="n">
-        <v>0.002109244622837149</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L8" t="n">
-        <v>0.003677057440048185</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M8" t="n">
-        <v>0.00209286825816626</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3028353265431929</v>
+        <v>0.1685526780378239</v>
       </c>
       <c r="O8" t="n">
-        <v>-0.254319494073837</v>
+        <v>0.0765745300688003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove pd.append function calls, get rid of gamma/kappa columns in scrambling input
</commit_message>
<xml_diff>
--- a/src/example_scrambling_output.xlsx
+++ b/src/example_scrambling_output.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ATM-B6" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="S2-B6" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ATM-B6" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ATM-S2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,23 +514,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003769909960995901</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007793352989302926</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002113201754037048</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003702305540019583</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0003887404917641695</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -551,10 +553,10 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2084769676046654</v>
+        <v>0.1826945278783137</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1160767438553549</v>
+        <v>0.09076446608354739</v>
       </c>
     </row>
     <row r="3">
@@ -587,25 +589,25 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.003720913787828295</v>
+        <v>0.003723787788712729</v>
       </c>
       <c r="J3" t="n">
-        <v>0.007734087273310928</v>
+        <v>0.007744018133863363</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002102735184248351</v>
+        <v>0.002106521197767294</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003673164546190823</v>
+        <v>0.003677948519669682</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0003877641643389194</v>
+        <v>0.0003881208956607774</v>
       </c>
       <c r="N3" t="n">
-        <v>0.173005804283726</v>
+        <v>0.1833394269032388</v>
       </c>
       <c r="O3" t="n">
-        <v>0.07992939702573887</v>
+        <v>0.09076888152995703</v>
       </c>
     </row>
     <row r="4">
@@ -653,10 +655,10 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1770877874050666</v>
+        <v>0.1830362050065858</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08469559471030816</v>
+        <v>0.09076680909892793</v>
       </c>
     </row>
     <row r="5">
@@ -669,50 +671,50 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003771759255797842</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00778260569127138</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002109276911031228</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003697117852169486</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003883691171730131</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.003720913787828295</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="J5" t="n">
-        <v>0.007734087273310928</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002102735184248351</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003673164546190823</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0003877641643389194</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="N5" t="n">
-        <v>0.141616624084127</v>
+        <v>0.1829611512843659</v>
       </c>
       <c r="O5" t="n">
-        <v>0.04854824788069214</v>
+        <v>0.09078368741430208</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>201207</v>
+        <v>201205</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -720,45 +722,45 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003775157024594888</v>
+        <v>0.003771759255797842</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007787727026405036</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002108787100421698</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003699702839221671</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G6" t="n">
-        <v>0.000388320234647194</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.003725249565827561</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007742350711306432</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002105977697171425</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003677140371788187</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0003880697129385161</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1496888401862124</v>
+        <v>0.1826902781350212</v>
       </c>
       <c r="O6" t="n">
-        <v>0.0577155186099103</v>
+        <v>0.09081304540795609</v>
       </c>
     </row>
     <row r="7">
@@ -771,96 +773,45 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.003767156216784404</v>
+        <v>0.003775157024594888</v>
       </c>
       <c r="D7" t="n">
-        <v>0.007780855852146149</v>
+        <v>0.007787727026405036</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002108585252719454</v>
+        <v>0.002108787100421698</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003696275723234606</v>
+        <v>0.003699702839221671</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0003883035805857967</v>
+        <v>0.000388320234647194</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0.003725249565827561</v>
+        <v>0.00373918479043579</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007742350711306432</v>
+        <v>0.007711495928810338</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002105977697171425</v>
+        <v>0.002085802198631657</v>
       </c>
       <c r="L7" t="n">
-        <v>0.003677140371788187</v>
+        <v>0.003662714003913901</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0003880697129385161</v>
+        <v>0.0003861730303119909</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2625447922510269</v>
+        <v>0.1821741353339218</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1705425960019301</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>201207</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.003774011943783199</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.007787067112526803</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.002110763953587128</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.003699278179158993</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0003885097115356922</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>B6</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0.003725249565827561</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.007742350711306432</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.002105977697171425</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.003677140371788187</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.0003880697129385161</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1685526780378239</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.0765745300688003</v>
+        <v>0.0908695026407999</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,6 +916,153 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.003723787788712729</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.007744018133863363</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.002106521197767294</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.003677948519669682</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0003881208956607774</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1826945278783137</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.09076446608354739</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>run_date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>15Rbulk_1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>17R_1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>15Rbulk_2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>17R_2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>ATM</t>
         </is>
       </c>
@@ -1004,10 +1102,10 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2084769676046654</v>
+        <v>0.1833394269032388</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1160767438553549</v>
+        <v>0.09076888152995703</v>
       </c>
     </row>
     <row r="3">
@@ -1020,50 +1118,248 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.003723787788712729</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.007744018133863363</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.002106521197767294</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.003677948519669682</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0003881208956607774</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1830362050065858</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.09076680909892793</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>run_date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>15Rbulk_1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>17R_1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ref_tag_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 31R_2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 45R_2</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>size corrected 46R_2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>15Rbulk_2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>17R_2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>kappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>0.003769909960995901</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1829611512843659</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.09078368741430208</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.003771759255797842</v>
+      </c>
       <c r="D3" t="n">
-        <v>0.007793352989302926</v>
+        <v>0.00778260569127138</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002113201754037048</v>
+        <v>0.002109276911031228</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003702305540019583</v>
+        <v>0.003697117852169486</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003887404917641695</v>
+        <v>0.0003883691171730131</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.003720913787828295</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="J3" t="n">
-        <v>0.007734087273310928</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002102735184248351</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003673164546190823</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0003877641643389194</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="N3" t="n">
-        <v>0.173005804283726</v>
+        <v>0.1826902781350212</v>
       </c>
       <c r="O3" t="n">
-        <v>0.07992939702573887</v>
+        <v>0.09081304540795609</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>201205</v>
+        <v>201207</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1071,249 +1367,45 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.003771759255797842</v>
+        <v>0.003775157024594888</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00778260569127138</v>
+        <v>0.007787727026405036</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002109276911031228</v>
+        <v>0.002108787100421698</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003697117852169486</v>
+        <v>0.003699702839221671</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0003883691171730131</v>
+        <v>0.000388320234647194</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>B6</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.003723787788712729</v>
+        <v>0.00373918479043579</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007744018133863363</v>
+        <v>0.007711495928810338</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002106521197767294</v>
+        <v>0.002085802198631657</v>
       </c>
       <c r="L4" t="n">
-        <v>0.003677948519669682</v>
+        <v>0.003662714003913901</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0003881208956607774</v>
+        <v>0.0003861730303119909</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1770877874050666</v>
+        <v>0.1821741353339218</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08469559471030816</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>201205</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.003771759255797842</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.00778260569127138</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.002109276911031228</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.003697117852169486</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.0003883691171730131</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>B6</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>0.003720913787828295</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.007734087273310928</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.002102735184248351</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.003673164546190823</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.0003877641643389194</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.141616624084127</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.04854824788069214</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>201207</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.003775157024594888</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.007787727026405036</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.002108787100421698</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.003699702839221671</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.000388320234647194</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>B6</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>0.003725249565827561</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.007742350711306432</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.002105977697171425</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.003677140371788187</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.0003880697129385161</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.1496888401862124</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.0577155186099103</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>201207</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.003767156216784404</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.007780855852146149</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.002108585252719454</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.003696275723234606</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0003883035805857967</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>B6</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>0.003725249565827561</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.007742350711306432</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.002105977697171425</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.003677140371788187</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.0003880697129385161</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.2625447922510269</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.1705425960019301</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>201207</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.003774011943783199</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.007787067112526803</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.002110763953587128</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.003699278179158993</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.0003885097115356922</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>B6</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0.003725249565827561</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.007742350711306432</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.002105977697171425</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.003677140371788187</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.0003880697129385161</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1685526780378239</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.0765745300688003</v>
+        <v>0.0908695026407999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not finding solution for SUP05 samples
</commit_message>
<xml_diff>
--- a/src/example_scrambling_output.xlsx
+++ b/src/example_scrambling_output.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,19 +518,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003738643261235055</v>
+        <v>0.003739233088364244</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007713298460153434</v>
+        <v>0.007713771018955469</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002088521517010378</v>
+        <v>0.00208815570518581</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003663482298378412</v>
+        <v>0.003663733992224545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0003864278685440451</v>
+        <v>0.000386393261386031</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -553,10 +553,10 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1826945278783137</v>
+        <v>0.1826091574760936</v>
       </c>
       <c r="O2" t="n">
-        <v>0.09076446608354739</v>
+        <v>0.09076378674752286</v>
       </c>
     </row>
     <row r="3">
@@ -565,23 +565,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.003769909960995901</v>
+        <v>0.003739233088364244</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007793352989302926</v>
+        <v>0.007713771018955469</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002113201754037048</v>
+        <v>0.00208815570518581</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003702305540019583</v>
+        <v>0.003663733992224545</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003887404917641695</v>
+        <v>0.000386393261386031</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -589,25 +589,25 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>0.003723787788712729</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J3" t="n">
-        <v>0.007744018133863363</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K3" t="n">
-        <v>0.002106521197767294</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L3" t="n">
-        <v>0.003677948519669682</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0003881208956607774</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1833394269032388</v>
+        <v>0.1828797011034304</v>
       </c>
       <c r="O3" t="n">
-        <v>0.09076888152995703</v>
+        <v>0.09069364405873254</v>
       </c>
     </row>
     <row r="4">
@@ -616,23 +616,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.003771759255797842</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00778260569127138</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002109276911031228</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="F4" t="n">
-        <v>0.003697117852169486</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0003883691171730131</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -655,10 +655,10 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1830362050065858</v>
+        <v>0.1826945278783137</v>
       </c>
       <c r="O4" t="n">
-        <v>0.09076680909892793</v>
+        <v>0.09076446608354739</v>
       </c>
     </row>
     <row r="5">
@@ -667,100 +667,100 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.003769909960995901</v>
+        <v>0.003738643261235055</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007793352989302926</v>
+        <v>0.007713298460153434</v>
       </c>
       <c r="E5" t="n">
-        <v>0.002113201754037048</v>
+        <v>0.002088521517010378</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003702305540019583</v>
+        <v>0.003663482298378412</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003887404917641695</v>
+        <v>0.0003864278685440451</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>B6</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.003738643261235055</v>
+        <v>0.003720913787828295</v>
       </c>
       <c r="J5" t="n">
-        <v>0.007713298460153434</v>
+        <v>0.007734087273310928</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002088521517010378</v>
+        <v>0.002102735184248351</v>
       </c>
       <c r="L5" t="n">
-        <v>0.003663482298378412</v>
+        <v>0.003673164546190823</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0003864278685440451</v>
+        <v>0.0003877641643389194</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1829611512843659</v>
+        <v>0.1829650630797686</v>
       </c>
       <c r="O5" t="n">
-        <v>0.09078368741430208</v>
+        <v>0.09069431689379176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>201205</v>
+        <v>201207</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.003771759255797842</v>
+        <v>0.00373918479043579</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00778260569127138</v>
+        <v>0.007711495928810338</v>
       </c>
       <c r="E6" t="n">
-        <v>0.002109276911031228</v>
+        <v>0.002085802198631657</v>
       </c>
       <c r="F6" t="n">
-        <v>0.003697117852169486</v>
+        <v>0.003662714003913901</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0003883691171730131</v>
+        <v>0.0003861730303119909</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>B6</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0.003738643261235055</v>
+        <v>0.003725249565827561</v>
       </c>
       <c r="J6" t="n">
-        <v>0.007713298460153434</v>
+        <v>0.007742350711306432</v>
       </c>
       <c r="K6" t="n">
-        <v>0.002088521517010378</v>
+        <v>0.002105977697171425</v>
       </c>
       <c r="L6" t="n">
-        <v>0.003663482298378412</v>
+        <v>0.003677140371788187</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0003864278685440451</v>
+        <v>0.0003880697129385161</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1826902781350212</v>
+        <v>0.1824232964537167</v>
       </c>
       <c r="O6" t="n">
-        <v>0.09081304540795609</v>
+        <v>0.09080601590571159</v>
       </c>
     </row>
     <row r="7">
@@ -769,49 +769,916 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="C7" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1823989500562382</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.09080581298183776</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003769909960995901</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0.003723787788712729</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.007744018133863363</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.002106521197767294</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.003677948519669682</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0003881208956607774</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1833394269032388</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.09076888152995703</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.003769909960995901</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1836060773700326</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.09069827494716363</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0.003723787788712729</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.007744018133863363</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.002106521197767294</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.003677948519669682</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0003881208956607774</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1830362050065858</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.09076680909892793</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1833028773867317</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.09069621748200445</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>0.003775157024594888</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D12" t="n">
         <v>0.007787727026405036</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E12" t="n">
         <v>0.002108787100421698</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F12" t="n">
         <v>0.003699702839221671</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G12" t="n">
         <v>0.000388320234647194</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.1824047520954045</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.09080549263438215</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.1834953658609197</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.09081333996010488</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.1825874080828793</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.09080715936119879</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.003769909960995901</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>S2</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="I15" t="n">
+        <v>0.003739233088364244</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.007713771018955469</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.00208815570518581</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.003663733992224545</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.000386393261386031</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.182886119565302</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.09079223885947683</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.003769909960995901</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1829611512843659</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.09078368741430208</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>0.003739233088364244</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.007713771018955469</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.00208815570518581</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.003663733992224545</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.000386393261386031</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.1826152448674723</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.09082159706479563</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1826902781350212</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.09081304540795609</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.003775157024594888</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.007787727026405036</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.002108787100421698</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.003699702839221671</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.000388320234647194</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
         <v>0.00373918479043579</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J19" t="n">
         <v>0.007711495928810338</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K19" t="n">
         <v>0.002085802198631657</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L19" t="n">
         <v>0.003662714003913901</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M19" t="n">
         <v>0.0003861730303119909</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N19" t="n">
         <v>0.1821741353339218</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O19" t="n">
         <v>0.0908695026407999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.003775157024594888</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.007787727026405036</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.002108787100421698</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.003699702839221671</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.000388320234647194</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.1821527448253449</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.09087194078298577</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>0.00373918479043579</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.007711495928810338</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.002085802198631657</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.003662714003913901</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.0003861730303119909</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.1831480486383229</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.09076395560935356</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.183126660185694</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.09076639394059735</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0.00373918479043579</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.007711495928810338</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.002085802198631657</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.003662714003913901</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.0003861730303119909</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.1823369396284753</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.09085186742092939</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.1823155494265338</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.09085430554016978</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +1692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,19 +1787,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003738643261235055</v>
+        <v>0.003739233088364244</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007713298460153434</v>
+        <v>0.007713771018955469</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002088521517010378</v>
+        <v>0.00208815570518581</v>
       </c>
       <c r="F2" t="n">
-        <v>0.003663482298378412</v>
+        <v>0.003663733992224545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0003864278685440451</v>
+        <v>0.000386393261386031</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -955,10 +1822,265 @@
         <v>0.0003881208956607774</v>
       </c>
       <c r="N2" t="n">
+        <v>0.1826091574760936</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.09076378674752286</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.003739233088364244</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.007713771018955469</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00208815570518581</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.003663733992224545</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.000386393261386031</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1828797011034304</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.09069364405873254</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.003723787788712729</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.007744018133863363</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.002106521197767294</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.003677948519669682</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0003881208956607774</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.1826945278783137</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O4" t="n">
         <v>0.09076446608354739</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1829650630797686</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.09069431689379176</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.00373918479043579</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.007711495928810338</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.002085802198631657</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.003662714003913901</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0003861730303119909</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.1824232964537167</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.09080601590571159</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1823989500562382</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.09080581298183776</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +2094,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1118,45 +2240,300 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>0.003769909960995901</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.007793352989302926</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.002113201754037048</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.003702305540019583</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0003887404917641695</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.1836060773700326</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.09069827494716363</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>0.003771759255797842</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>0.00778260569127138</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E4" t="n">
         <v>0.002109276911031228</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F4" t="n">
         <v>0.003697117852169486</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G4" t="n">
         <v>0.0003883691171730131</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>B6</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="I4" t="n">
         <v>0.003723787788712729</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J4" t="n">
         <v>0.007744018133863363</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K4" t="n">
         <v>0.002106521197767294</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L4" t="n">
         <v>0.003677948519669682</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M4" t="n">
         <v>0.0003881208956607774</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N4" t="n">
         <v>0.1830362050065858</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O4" t="n">
         <v>0.09076680909892793</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.003720913787828295</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.007734087273310928</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.002102735184248351</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.003673164546190823</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0003877641643389194</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1833028773867317</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.09069621748200445</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.003775157024594888</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.007787727026405036</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.002108787100421698</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.003699702839221671</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.000388320234647194</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.1824047520954045</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.09080549263438215</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1834953658609197</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.09081333996010488</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0.003725249565827561</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.007742350711306432</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.002105977697171425</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.003677140371788187</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0003880697129385161</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1825874080828793</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.09080715936119879</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +2547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1285,25 +2662,25 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0.003738643261235055</v>
+        <v>0.003739233088364244</v>
       </c>
       <c r="J2" t="n">
-        <v>0.007713298460153434</v>
+        <v>0.007713771018955469</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002088521517010378</v>
+        <v>0.00208815570518581</v>
       </c>
       <c r="L2" t="n">
-        <v>0.003663482298378412</v>
+        <v>0.003663733992224545</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0003864278685440451</v>
+        <v>0.000386393261386031</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1829611512843659</v>
+        <v>0.182886119565302</v>
       </c>
       <c r="O2" t="n">
-        <v>0.09078368741430208</v>
+        <v>0.09079223885947683</v>
       </c>
     </row>
     <row r="3">
@@ -1316,19 +2693,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.003771759255797842</v>
+        <v>0.003769909960995901</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00778260569127138</v>
+        <v>0.007793352989302926</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002109276911031228</v>
+        <v>0.002113201754037048</v>
       </c>
       <c r="F3" t="n">
-        <v>0.003697117852169486</v>
+        <v>0.003702305540019583</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0003883691171730131</v>
+        <v>0.0003887404917641695</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1351,61 +2728,418 @@
         <v>0.0003864278685440451</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1826902781350212</v>
+        <v>0.1829611512843659</v>
       </c>
       <c r="O3" t="n">
-        <v>0.09081304540795609</v>
+        <v>0.09078368741430208</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.003739233088364244</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.007713771018955469</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.00208815570518581</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.003663733992224545</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.000386393261386031</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.1826152448674723</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.09082159706479563</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>201205</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.003771759255797842</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.00778260569127138</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.002109276911031228</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.003697117852169486</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0003883691171730131</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.003738643261235055</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.007713298460153434</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.002088521517010378</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.003663482298378412</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0003864278685440451</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1826902781350212</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.09081304540795609</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>201207</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>0.003775157024594888</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D6" t="n">
         <v>0.007787727026405036</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E6" t="n">
         <v>0.002108787100421698</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F6" t="n">
         <v>0.003699702839221671</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G6" t="n">
         <v>0.000388320234647194</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>S2</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I6" t="n">
         <v>0.00373918479043579</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J6" t="n">
         <v>0.007711495928810338</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K6" t="n">
         <v>0.002085802198631657</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L6" t="n">
         <v>0.003662714003913901</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M6" t="n">
         <v>0.0003861730303119909</v>
       </c>
-      <c r="N4" t="n">
+      <c r="N6" t="n">
         <v>0.1821741353339218</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O6" t="n">
         <v>0.0908695026407999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.003775157024594888</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.007787727026405036</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002108787100421698</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.003699702839221671</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.000388320234647194</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1821527448253449</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.09087194078298577</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0.00373918479043579</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.007711495928810338</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.002085802198631657</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.003662714003913901</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0003861730303119909</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.1831480486383229</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.09076395560935356</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.003767156216784404</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.007780855852146149</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002108585252719454</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.003696275723234606</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0003883035805857967</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.183126660185694</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.09076639394059735</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0.00373918479043579</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.007711495928810338</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.002085802198631657</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.003662714003913901</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0003861730303119909</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1823369396284753</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.09085186742092939</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>201207</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ATM</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.003774011943783199</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.007787067112526803</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002110763953587128</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.003699278179158993</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0003885097115356922</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0.003739541106399988</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.007710852308599518</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.002087697164321905</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.003662306506347789</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0003863513375294824</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1823155494265338</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.09085430554016978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add check 31R script and 31R error columns to scrambling calculation
</commit_message>
<xml_diff>
--- a/src/example_scrambling_output.xlsx
+++ b/src/example_scrambling_output.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,16 @@
           <t>kappa</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref1_permil</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref2_permil</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -558,6 +568,12 @@
       <c r="O2" t="n">
         <v>0.09076378674752286</v>
       </c>
+      <c r="P2" t="n">
+        <v>-0.4091049258002633</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.4091049258002633</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -609,6 +625,12 @@
       <c r="O3" t="n">
         <v>0.09069364405873254</v>
       </c>
+      <c r="P3" t="n">
+        <v>-0.7444554516042867</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.7444554516042867</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -660,6 +682,12 @@
       <c r="O4" t="n">
         <v>0.09076446608354739</v>
       </c>
+      <c r="P4" t="n">
+        <v>-0.3258536615019514</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.3258536615019514</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -711,6 +739,12 @@
       <c r="O5" t="n">
         <v>0.09069431689379176</v>
       </c>
+      <c r="P5" t="n">
+        <v>-0.661254864741001</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.661254864741001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -762,6 +796,12 @@
       <c r="O6" t="n">
         <v>0.09080601590571159</v>
       </c>
+      <c r="P6" t="n">
+        <v>-0.2304847950564959</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.2304847950564959</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -813,6 +853,12 @@
       <c r="O7" t="n">
         <v>0.09080581298183776</v>
       </c>
+      <c r="P7" t="n">
+        <v>-0.2542075049479786</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.2542075049479786</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -864,6 +910,12 @@
       <c r="O8" t="n">
         <v>0.09076888152995703</v>
       </c>
+      <c r="P8" t="n">
+        <v>0.3000358365834455</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.3000358365834455</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -915,6 +967,12 @@
       <c r="O9" t="n">
         <v>0.09069827494716363</v>
       </c>
+      <c r="P9" t="n">
+        <v>-0.03250962188272588</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-0.03250962188272588</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -966,6 +1024,12 @@
       <c r="O10" t="n">
         <v>0.09076680909892793</v>
       </c>
+      <c r="P10" t="n">
+        <v>0.009129185265965845</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.009129185265965845</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1017,6 +1081,12 @@
       <c r="O11" t="n">
         <v>0.09069621748200445</v>
       </c>
+      <c r="P11" t="n">
+        <v>-0.3232611217129921</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-0.3232611217129921</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1068,6 +1138,12 @@
       <c r="O12" t="n">
         <v>0.09080549263438215</v>
       </c>
+      <c r="P12" t="n">
+        <v>-0.2421222941543233</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-0.2421222941543233</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1119,6 +1195,12 @@
       <c r="O13" t="n">
         <v>0.09081333996010488</v>
       </c>
+      <c r="P13" t="n">
+        <v>0.804003732371994</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.804003732371994</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1170,6 +1252,12 @@
       <c r="O14" t="n">
         <v>0.09080715936119879</v>
       </c>
+      <c r="P14" t="n">
+        <v>-0.06757790660705254</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-0.06757790660705254</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1221,6 +1309,12 @@
       <c r="O15" t="n">
         <v>0.09079223885947683</v>
       </c>
+      <c r="P15" t="n">
+        <v>0.7714581516891084</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.7714581516891084</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1272,6 +1366,12 @@
       <c r="O16" t="n">
         <v>0.09078368741430208</v>
       </c>
+      <c r="P16" t="n">
+        <v>0.68887662279149</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.68887662279149</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1323,6 +1423,12 @@
       <c r="O17" t="n">
         <v>0.09082159706479563</v>
       </c>
+      <c r="P17" t="n">
+        <v>0.4788328094882388</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.4788328094882388</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1374,6 +1480,12 @@
       <c r="O18" t="n">
         <v>0.09081304540795609</v>
       </c>
+      <c r="P18" t="n">
+        <v>0.3962898487157585</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.3962898487157585</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1425,6 +1537,12 @@
       <c r="O19" t="n">
         <v>0.0908695026407999</v>
       </c>
+      <c r="P19" t="n">
+        <v>0.04794438160171666</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.04794438160171666</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1476,6 +1594,12 @@
       <c r="O20" t="n">
         <v>0.09087194078298577</v>
       </c>
+      <c r="P20" t="n">
+        <v>0.07145489776094749</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.07145489776094749</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1527,6 +1651,12 @@
       <c r="O21" t="n">
         <v>0.09076395560935356</v>
       </c>
+      <c r="P21" t="n">
+        <v>1.100060574029005</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1.100060574029005</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1578,6 +1708,12 @@
       <c r="O22" t="n">
         <v>0.09076639394059735</v>
       </c>
+      <c r="P22" t="n">
+        <v>1.123618980839014</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1.123618980839014</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1629,6 +1765,12 @@
       <c r="O23" t="n">
         <v>0.09085186742092939</v>
       </c>
+      <c r="P23" t="n">
+        <v>0.2234770376519091</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.2234770376519091</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1679,6 +1821,12 @@
       </c>
       <c r="O24" t="n">
         <v>0.09085430554016978</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.2469943301994793</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.2469943301994793</v>
       </c>
     </row>
   </sheetData>
@@ -1692,7 +1840,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1776,6 +1924,16 @@
           <t>kappa</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref1_permil</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref2_permil</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1827,6 +1985,12 @@
       <c r="O2" t="n">
         <v>0.09076378674752286</v>
       </c>
+      <c r="P2" t="n">
+        <v>-0.4091049258002633</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.4091049258002633</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1878,6 +2042,12 @@
       <c r="O3" t="n">
         <v>0.09069364405873254</v>
       </c>
+      <c r="P3" t="n">
+        <v>-0.7444554516042867</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.7444554516042867</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1929,6 +2099,12 @@
       <c r="O4" t="n">
         <v>0.09076446608354739</v>
       </c>
+      <c r="P4" t="n">
+        <v>-0.3258536615019514</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.3258536615019514</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1980,6 +2156,12 @@
       <c r="O5" t="n">
         <v>0.09069431689379176</v>
       </c>
+      <c r="P5" t="n">
+        <v>-0.661254864741001</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.661254864741001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2031,6 +2213,12 @@
       <c r="O6" t="n">
         <v>0.09080601590571159</v>
       </c>
+      <c r="P6" t="n">
+        <v>-0.2304847950564959</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.2304847950564959</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2081,6 +2269,12 @@
       </c>
       <c r="O7" t="n">
         <v>0.09080581298183776</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-0.2542075049479786</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.2542075049479786</v>
       </c>
     </row>
   </sheetData>
@@ -2094,7 +2288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2178,6 +2372,16 @@
           <t>kappa</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref1_permil</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref2_permil</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2229,6 +2433,12 @@
       <c r="O2" t="n">
         <v>0.09076888152995703</v>
       </c>
+      <c r="P2" t="n">
+        <v>0.3000358365834455</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.3000358365834455</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2280,6 +2490,12 @@
       <c r="O3" t="n">
         <v>0.09069827494716363</v>
       </c>
+      <c r="P3" t="n">
+        <v>-0.03250962188272588</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.03250962188272588</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2331,6 +2547,12 @@
       <c r="O4" t="n">
         <v>0.09076680909892793</v>
       </c>
+      <c r="P4" t="n">
+        <v>0.009129185265965845</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.009129185265965845</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2382,6 +2604,12 @@
       <c r="O5" t="n">
         <v>0.09069621748200445</v>
       </c>
+      <c r="P5" t="n">
+        <v>-0.3232611217129921</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.3232611217129921</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2433,6 +2661,12 @@
       <c r="O6" t="n">
         <v>0.09080549263438215</v>
       </c>
+      <c r="P6" t="n">
+        <v>-0.2421222941543233</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-0.2421222941543233</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2484,6 +2718,12 @@
       <c r="O7" t="n">
         <v>0.09081333996010488</v>
       </c>
+      <c r="P7" t="n">
+        <v>0.804003732371994</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.804003732371994</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2534,6 +2774,12 @@
       </c>
       <c r="O8" t="n">
         <v>0.09080715936119879</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.06757790660705254</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-0.06757790660705254</v>
       </c>
     </row>
   </sheetData>
@@ -2547,7 +2793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2631,6 +2877,16 @@
           <t>kappa</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref1_permil</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>error31r_ref2_permil</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2682,6 +2938,12 @@
       <c r="O2" t="n">
         <v>0.09079223885947683</v>
       </c>
+      <c r="P2" t="n">
+        <v>0.7714581516891084</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.7714581516891084</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2733,6 +2995,12 @@
       <c r="O3" t="n">
         <v>0.09078368741430208</v>
       </c>
+      <c r="P3" t="n">
+        <v>0.68887662279149</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.68887662279149</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2784,6 +3052,12 @@
       <c r="O4" t="n">
         <v>0.09082159706479563</v>
       </c>
+      <c r="P4" t="n">
+        <v>0.4788328094882388</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.4788328094882388</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2835,6 +3109,12 @@
       <c r="O5" t="n">
         <v>0.09081304540795609</v>
       </c>
+      <c r="P5" t="n">
+        <v>0.3962898487157585</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.3962898487157585</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2886,6 +3166,12 @@
       <c r="O6" t="n">
         <v>0.0908695026407999</v>
       </c>
+      <c r="P6" t="n">
+        <v>0.04794438160171666</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.04794438160171666</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2937,6 +3223,12 @@
       <c r="O7" t="n">
         <v>0.09087194078298577</v>
       </c>
+      <c r="P7" t="n">
+        <v>0.07145489776094749</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.07145489776094749</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2988,6 +3280,12 @@
       <c r="O8" t="n">
         <v>0.09076395560935356</v>
       </c>
+      <c r="P8" t="n">
+        <v>1.100060574029005</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.100060574029005</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -3039,6 +3337,12 @@
       <c r="O9" t="n">
         <v>0.09076639394059735</v>
       </c>
+      <c r="P9" t="n">
+        <v>1.123618980839014</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.123618980839014</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -3090,6 +3394,12 @@
       <c r="O10" t="n">
         <v>0.09085186742092939</v>
       </c>
+      <c r="P10" t="n">
+        <v>0.2234770376519091</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.2234770376519091</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -3140,6 +3450,12 @@
       </c>
       <c r="O11" t="n">
         <v>0.09085430554016978</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.2469943301994793</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.2469943301994793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>